<commit_message>
Make nicer Graphs for EncoderData
Done in Mrs. Neuman's class :+1: If @pandapig12 would print this off for Alexander that would be nice
</commit_message>
<xml_diff>
--- a/EncoderData.xlsx
+++ b/EncoderData.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ECohen\Desktop\CODE\FTC-2015\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wjackson\Desktop\FTC-2015\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8115" xr2:uid="{8701EB1F-E7F2-45FF-B410-39A3A3FA6C22}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="8112" xr2:uid="{8701EB1F-E7F2-45FF-B410-39A3A3FA6C22}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Left</t>
   </si>
@@ -48,6 +48,12 @@
   </si>
   <si>
     <t>STDEV</t>
+  </si>
+  <si>
+    <t>Error per meter (cm)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -100,6 +106,1034 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Ticks</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> per centimeter values</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Left ticks per cm</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$2:$E$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>25.382121352477998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>25.105557457491727</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>24.499437570303712</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>25.810560444650303</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25.94951366373321</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25.607668606641564</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>25.590551181102359</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>24.856964821843313</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>25.312644742936545</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>25.208262010726923</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000C-F908-4261-A051-869BAB7C3447}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Right ticks per cm</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$F$2:$F$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>25.138953219082907</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>24.888736733995209</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>25.658042744656917</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>25.509495136637334</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25.752663270032421</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25.436494351249575</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>25.388076490438692</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>24.573726845295418</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>25.081056044465029</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>24.980029670204271</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000D-F908-4261-A051-869BAB7C3447}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="302368040"/>
+        <c:axId val="378484080"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="302368040"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="378484080"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="378484080"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="302368040"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>327660</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>102870</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>53340</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D3218CE0-583F-491D-911A-DDD23CE16C16}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -399,19 +1433,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54E30C7B-F6E3-44F2-B7FF-3EAAA2094733}">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="9.28515625" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.33203125" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -431,7 +1465,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2192</v>
       </c>
@@ -442,19 +1476,19 @@
         <v>34</v>
       </c>
       <c r="D2">
-        <f>C2*2.54</f>
+        <f t="shared" ref="D2:D11" si="0">C2*2.54</f>
         <v>86.36</v>
       </c>
       <c r="E2">
-        <f>A2/D2</f>
+        <f t="shared" ref="E2:E11" si="1">A2/D2</f>
         <v>25.382121352477998</v>
       </c>
       <c r="F2">
-        <f>B2/D2</f>
+        <f t="shared" ref="F2:F11" si="2">B2/D2</f>
         <v>25.138953219082907</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2200</v>
       </c>
@@ -465,19 +1499,19 @@
         <v>34.5</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D11" si="0">C3*2.54</f>
+        <f t="shared" si="0"/>
         <v>87.63</v>
       </c>
       <c r="E3">
-        <f>A3/D3</f>
+        <f t="shared" si="1"/>
         <v>25.105557457491727</v>
       </c>
       <c r="F3">
-        <f>B3/D3</f>
+        <f t="shared" si="2"/>
         <v>24.888736733995209</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2178</v>
       </c>
@@ -492,15 +1526,15 @@
         <v>88.9</v>
       </c>
       <c r="E4">
-        <f t="shared" ref="E4:E11" si="1">A4/D4</f>
+        <f t="shared" si="1"/>
         <v>24.499437570303712</v>
       </c>
       <c r="F4">
-        <f t="shared" ref="F4:F11" si="2">B4/D4</f>
+        <f t="shared" si="2"/>
         <v>25.658042744656917</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2229</v>
       </c>
@@ -523,7 +1557,7 @@
         <v>25.509495136637334</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2241</v>
       </c>
@@ -546,7 +1580,7 @@
         <v>25.752663270032421</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2244</v>
       </c>
@@ -569,7 +1603,7 @@
         <v>25.436494351249575</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>2275</v>
       </c>
@@ -592,7 +1626,7 @@
         <v>25.388076490438692</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2194</v>
       </c>
@@ -615,7 +1649,7 @@
         <v>24.573726845295418</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>2186</v>
       </c>
@@ -638,7 +1672,7 @@
         <v>25.081056044465029</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>2209</v>
       </c>
@@ -661,7 +1695,7 @@
         <v>24.980029670204271</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -674,7 +1708,7 @@
         <v>25.240727450605778</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -687,7 +1721,27 @@
         <v>0.37134984744171279</v>
       </c>
     </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14">
+        <f>100*E13/E12</f>
+        <v>1.73645078965602</v>
+      </c>
+      <c r="F14">
+        <f>100*F13/F12</f>
+        <v>1.4712327454445073</v>
+      </c>
+    </row>
+    <row r="24" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E24" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>